<commit_message>
COMPLETELY FINALIZED THE PROJECT
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/Suite.xlsx
+++ b/src/test/resources/excel/Suite.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\polan\IdeaProjects\PageObjectModel\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Playwright Java\New folder\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D351071A-3878-44BE-B79E-19E11409CCD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1335F77-2E46-4A0D-AE83-5FCB3372F2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suite" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>SuiteName</t>
   </si>
@@ -28,13 +28,7 @@
     <t>Runmode</t>
   </si>
   <si>
-    <t>BankManagerSuite</t>
-  </si>
-  <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>CustomerSuite</t>
   </si>
   <si>
     <t>CarWaleSuite</t>
@@ -79,8 +73,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -302,15 +296,15 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A3" sqref="A3:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -318,29 +312,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>